<commit_message>
Finished CppCon 2016 talk
</commit_message>
<xml_diff>
--- a/graphs/benchmark_locking core count comparison.xlsx
+++ b/graphs/benchmark_locking core count comparison.xlsx
@@ -63,7 +63,7 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:chart>
     <c:plotArea>
       <c:layout/>
@@ -734,24 +734,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="127702912"/>
-        <c:axId val="127704448"/>
+        <c:axId val="164861440"/>
+        <c:axId val="164862976"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="127702912"/>
+        <c:axId val="164861440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="127704448"/>
+        <c:crossAx val="164862976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="127704448"/>
+        <c:axId val="164862976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -759,7 +759,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="127702912"/>
+        <c:crossAx val="164861440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -772,7 +772,296 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-GB"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>How well each locking algorithm scales CONTENDED to doubling CPU core count on NTFS</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>lock files</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$7:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2.0614510037765852</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.633024633024633</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.3822717000083702</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.2639044255810723</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.192137830623635</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.1026412055479879</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.98586715122148183</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.93047960099566018</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>byte ranges</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$18:$B$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.6315244861586138</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.57871231179742111</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.89566533317185182</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.84652531350178184</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.87815095595333403</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.9138339878013676</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.94309205664739471</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.83525081072522611</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>atomic append</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$29:$B$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.94472993651710602</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0189215775700222</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.96150544081285605</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0235536067839184</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0272187433576216</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0348735880464779</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0494959569445543</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.98942844038054656</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>memory map</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$40:$B$47</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.86669364354482048</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.92450143819506436</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.88951126759309607</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0387976066996754</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.1338837827621675</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0092265840047945</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.93910436943821152</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.84588891572597869</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="161092352"/>
+        <c:axId val="161109120"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="161092352"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Concurrency</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="161109120"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="161109120"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Performance of quad core CPU relative to a dual core CPU</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="161092352"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1800"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -780,7 +1069,7 @@
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:chart>
     <c:plotArea>
       <c:layout/>
@@ -1451,24 +1740,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="128024960"/>
-        <c:axId val="128026496"/>
+        <c:axId val="165187584"/>
+        <c:axId val="165189120"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="128024960"/>
+        <c:axId val="165187584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="128026496"/>
+        <c:crossAx val="165189120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="128026496"/>
+        <c:axId val="165189120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1476,7 +1765,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="128024960"/>
+        <c:crossAx val="165187584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1489,7 +1778,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1497,7 +1786,7 @@
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:chart>
     <c:plotArea>
       <c:layout/>
@@ -2168,24 +2457,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="128089088"/>
-        <c:axId val="128103168"/>
+        <c:axId val="165255808"/>
+        <c:axId val="165261696"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="128089088"/>
+        <c:axId val="165255808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="128103168"/>
+        <c:crossAx val="165261696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="128103168"/>
+        <c:axId val="165261696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2193,7 +2482,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="128089088"/>
+        <c:crossAx val="165255808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2206,7 +2495,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2214,7 +2503,7 @@
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:chart>
     <c:plotArea>
       <c:layout/>
@@ -2885,24 +3174,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="128152704"/>
-        <c:axId val="128154240"/>
+        <c:axId val="164930304"/>
+        <c:axId val="164931840"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="128152704"/>
+        <c:axId val="164930304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="128154240"/>
+        <c:crossAx val="164931840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="128154240"/>
+        <c:axId val="164931840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2910,7 +3199,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="128152704"/>
+        <c:crossAx val="164930304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2923,7 +3212,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2931,7 +3220,7 @@
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:chart>
     <c:plotArea>
       <c:layout/>
@@ -3602,24 +3891,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="128200064"/>
-        <c:axId val="128222336"/>
+        <c:axId val="165428224"/>
+        <c:axId val="165454592"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="128200064"/>
+        <c:axId val="165428224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="128222336"/>
+        <c:crossAx val="165454592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="128222336"/>
+        <c:axId val="165454592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3627,7 +3916,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="128200064"/>
+        <c:crossAx val="165428224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3640,7 +3929,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3648,7 +3937,7 @@
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:chart>
     <c:plotArea>
       <c:layout/>
@@ -4319,24 +4608,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="128345984"/>
-        <c:axId val="128347520"/>
+        <c:axId val="165303808"/>
+        <c:axId val="165305344"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="128345984"/>
+        <c:axId val="165303808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="128347520"/>
+        <c:crossAx val="165305344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="128347520"/>
+        <c:axId val="165305344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4344,7 +4633,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="128345984"/>
+        <c:crossAx val="165303808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4357,7 +4646,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4365,7 +4654,7 @@
 
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:chart>
     <c:plotArea>
       <c:layout/>
@@ -5036,24 +5325,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="128274816"/>
-        <c:axId val="128276352"/>
+        <c:axId val="191651840"/>
+        <c:axId val="191653376"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="128274816"/>
+        <c:axId val="191651840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="128276352"/>
+        <c:crossAx val="191653376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="128276352"/>
+        <c:axId val="191653376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5061,7 +5350,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="128274816"/>
+        <c:crossAx val="191651840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5074,7 +5363,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5082,7 +5371,7 @@
 
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:chart>
     <c:plotArea>
       <c:layout/>
@@ -5753,24 +6042,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="128388096"/>
-        <c:axId val="128406272"/>
+        <c:axId val="191699584"/>
+        <c:axId val="191709568"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="128388096"/>
+        <c:axId val="191699584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="128406272"/>
+        <c:crossAx val="191709568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="128406272"/>
+        <c:axId val="191709568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5778,7 +6067,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="128388096"/>
+        <c:crossAx val="191699584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5791,7 +6080,296 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-GB"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>How well each locking algorithm scales UNCONTENDED to doubling CPU core count on NTFS</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>lock files</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$51:$B$58</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2.1426607081471296</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.3106319971108702</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.4492663483273809</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.6653510394825202</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.7816807469986657</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.6163061607252951</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.5857763920047661</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.3024397755269641</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>byte ranges</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$62:$B$69</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.6472478869405949</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5589947443525076</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.6153161459319352</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.516804808379167</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.3779775273874222</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.3131683064472262</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.2628964678574883</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.2074762667790755</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>atomic append</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$73:$B$80</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.97266678691946107</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.1495445473117898</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1929378314914705</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0655044364337454</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.96718505575978164</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0007623517911526</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.99365014615410197</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.98954338998971503</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>memory map</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$84:$B$91</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.80157129121296389</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0243804889831027</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1513468421156487</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.3428651512326177</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.5141316173513846</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.6893734184012654</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.8650468408693888</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.9341970698828861</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="161479680"/>
+        <c:axId val="46551808"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="161479680"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Concurrency</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="46551808"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="46551808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Performance of quad core CPU relative to a dual core CPU</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="161479680"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1800"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6034,6 +6612,66 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>600074</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>214874</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>78599</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="12" name="Chart 11"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>224400</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>145275</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="14" name="Chart 13"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -10635,8 +11273,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A5:AA91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="K54" sqref="K54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>